<commit_message>
All Hopper changes to date.
</commit_message>
<xml_diff>
--- a/Material density values.xlsx
+++ b/Material density values.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="16155" windowHeight="9975"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="16155" windowHeight="9975" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
   <si>
     <t>Material</t>
   </si>
@@ -64,6 +64,176 @@
   </si>
   <si>
     <t>5300 (probably 6600 and 6400)</t>
+  </si>
+  <si>
+    <t>Line</t>
+  </si>
+  <si>
+    <t>Extruder hopper
+prealarm number</t>
+  </si>
+  <si>
+    <t>Extruder hopper
+postalarm #</t>
+  </si>
+  <si>
+    <t>Materials</t>
+  </si>
+  <si>
+    <t>Densities</t>
+  </si>
+  <si>
+    <t>R01C-01</t>
+  </si>
+  <si>
+    <t>generic pp</t>
+  </si>
+  <si>
+    <t>K606</t>
+  </si>
+  <si>
+    <t>mfr data</t>
+  </si>
+  <si>
+    <t>Default gross</t>
+  </si>
+  <si>
+    <t>Time to drain</t>
+  </si>
+  <si>
+    <t>Percent/100</t>
+  </si>
+  <si>
+    <t>implied cube side</t>
+  </si>
+  <si>
+    <t>Capacity (lbs)</t>
+  </si>
+  <si>
+    <t>Listed capacity</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Capacity 5300</t>
+  </si>
+  <si>
+    <t>Blender+ hopper #</t>
+  </si>
+  <si>
+    <t>Only hopper #</t>
+  </si>
+  <si>
+    <t>ratio k606/pmx</t>
+  </si>
+  <si>
+    <t>predicted # 100% pmx</t>
+  </si>
+  <si>
+    <t>off by 4500</t>
+  </si>
+  <si>
+    <t>Hopper</t>
+  </si>
+  <si>
+    <t>6 Ex</t>
+  </si>
+  <si>
+    <t>6 Ex pre</t>
+  </si>
+  <si>
+    <t>6 Ex post</t>
+  </si>
+  <si>
+    <t>6 Ex + blend</t>
+  </si>
+  <si>
+    <t>6 1</t>
+  </si>
+  <si>
+    <t>6 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 3 </t>
+  </si>
+  <si>
+    <t>6 4</t>
+  </si>
+  <si>
+    <t>6 5</t>
+  </si>
+  <si>
+    <t>Pmx</t>
+  </si>
+  <si>
+    <t>Resin</t>
+  </si>
+  <si>
+    <t>22300-25000</t>
+  </si>
+  <si>
+    <t>12000-19000</t>
+  </si>
+  <si>
+    <t>4000-9000</t>
+  </si>
+  <si>
+    <t>*8000-9000</t>
+  </si>
+  <si>
+    <t>9000-12000</t>
+  </si>
+  <si>
+    <t>HGX/HiCal 40/60</t>
+  </si>
+  <si>
+    <t>15 minutes (you lose HiCal after 20, grind may protect you)</t>
+  </si>
+  <si>
+    <t>11 Ex</t>
+  </si>
+  <si>
+    <t>11 Ex pre</t>
+  </si>
+  <si>
+    <t>11 Ex post</t>
+  </si>
+  <si>
+    <t>11 2</t>
+  </si>
+  <si>
+    <t>11 1</t>
+  </si>
+  <si>
+    <t>11 3</t>
+  </si>
+  <si>
+    <t>11 4</t>
+  </si>
+  <si>
+    <t>*28000-30000</t>
+  </si>
+  <si>
+    <t>13500-16000</t>
+  </si>
+  <si>
+    <t>Pmx/resin 50</t>
+  </si>
+  <si>
+    <t>*23800</t>
+  </si>
+  <si>
+    <t>*31200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pmx/resin </t>
+  </si>
+  <si>
+    <t>pmx/resin 25</t>
+  </si>
+  <si>
+    <t>FINAL ANSWER</t>
   </si>
 </sst>
 </file>
@@ -99,8 +269,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,22 +575,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -423,8 +604,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
+    <row r="2" spans="1:10">
+      <c r="A2" s="1">
         <v>3414</v>
       </c>
       <c r="B2">
@@ -438,8 +619,8 @@
         <v>1.3421827092388962E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B3">
@@ -453,8 +634,8 @@
         <v>1.5792195638521876E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4">
@@ -468,8 +649,8 @@
         <v>1.6007683688170321E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
@@ -483,8 +664,8 @@
         <v>2.1302532908103581E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B6">
@@ -498,8 +679,8 @@
         <v>2.1733509007400474E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B7">
@@ -513,8 +694,8 @@
         <v>2.3149573333661695E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8">
@@ -528,8 +709,8 @@
         <v>2.3211141347846968E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B9">
@@ -542,9 +723,16 @@
         <f>IF(B9, B9/C9, "")</f>
         <v>2.588934996490623E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9">
+        <f>D13/D4</f>
+        <v>2.175624542465</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
@@ -557,9 +745,19 @@
         <f>IF(B10, B10/C10, "")</f>
         <v>2.8321286525224417E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+      <c r="G10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10">
+        <f>36000/J9</f>
+        <v>16546.972741542853</v>
+      </c>
+      <c r="I10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11">
@@ -573,79 +771,94 @@
         <v>2.9891270886948811E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
+    <row r="12" spans="1:10">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>16.2422</v>
+      </c>
+      <c r="D12">
+        <v>3.2514562800000001E-2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13">
+        <v>16.2422</v>
+      </c>
+      <c r="D13">
+        <v>3.4826709499999997E-2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1">
+        <v>484</v>
+      </c>
+      <c r="C14">
+        <v>16.2422</v>
+      </c>
+      <c r="D14">
+        <v>3.7600000000000001E-2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B12">
+      <c r="B15">
         <v>0.69850000000000001</v>
       </c>
-      <c r="C12">
-        <v>16.2422</v>
-      </c>
-      <c r="D12">
-        <f>IF(B12, B12/C12, "")</f>
+      <c r="C15">
+        <v>16.2422</v>
+      </c>
+      <c r="D15">
+        <f>IF(B15, B15/C15, "")</f>
         <v>4.3005257908411421E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
+    <row r="16" spans="1:10">
+      <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B13">
+      <c r="B16">
         <v>0.74450000000000005</v>
       </c>
-      <c r="C13">
-        <v>16.2422</v>
-      </c>
-      <c r="D13">
-        <f>IF(B13, B13/C13, "")</f>
+      <c r="C16">
+        <v>16.2422</v>
+      </c>
+      <c r="D16">
+        <f>IF(B16, B16/C16, "")</f>
         <v>4.5837386560933863E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B14">
+      <c r="B17">
         <v>0.74450000000000005</v>
       </c>
-      <c r="C14">
-        <v>16.2422</v>
-      </c>
-      <c r="D14">
-        <f>IF(B14, B14/C14, "")</f>
+      <c r="C17">
+        <v>16.2422</v>
+      </c>
+      <c r="D17">
+        <f>IF(B17, B17/C17, "")</f>
         <v>4.5837386560933863E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="C15">
-        <v>16.2422</v>
-      </c>
-      <c r="D15" t="str">
-        <f>IF(B15, B15/C15, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="C16">
-        <v>16.2422</v>
-      </c>
-      <c r="D16" t="str">
-        <f>IF(B16, B16/C16, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="3:4">
-      <c r="C17">
-        <v>16.2422</v>
-      </c>
-      <c r="D17" t="str">
-        <f>IF(B17, B17/C17, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="3:4">
+    <row r="18" spans="1:4">
       <c r="C18">
         <v>16.2422</v>
       </c>
@@ -654,7 +867,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="3:4">
+    <row r="19" spans="1:4">
       <c r="C19">
         <v>16.2422</v>
       </c>
@@ -663,7 +876,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="3:4">
+    <row r="20" spans="1:4">
       <c r="C20">
         <v>16.2422</v>
       </c>
@@ -672,7 +885,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="3:4">
+    <row r="21" spans="1:4">
       <c r="C21">
         <v>16.2422</v>
       </c>
@@ -681,7 +894,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="3:4">
+    <row r="22" spans="1:4">
       <c r="C22">
         <v>16.2422</v>
       </c>
@@ -690,7 +903,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="3:4">
+    <row r="23" spans="1:4">
       <c r="C23">
         <v>16.2422</v>
       </c>
@@ -699,7 +912,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="3:4">
+    <row r="24" spans="1:4">
       <c r="C24">
         <v>16.2422</v>
       </c>
@@ -708,7 +921,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="3:4">
+    <row r="25" spans="1:4">
       <c r="C25">
         <v>16.2422</v>
       </c>
@@ -717,7 +930,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="3:4">
+    <row r="26" spans="1:4">
       <c r="C26">
         <v>16.2422</v>
       </c>
@@ -726,17 +939,8 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="3:4">
-      <c r="C27">
-        <v>16.2422</v>
-      </c>
-      <c r="D27" t="str">
-        <f>IF(B27, B27/C27, "")</f>
-        <v/>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A2:D27">
+  <sortState ref="A2:E27">
     <sortCondition ref="D2:D27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -745,24 +949,668 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="12.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="30" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="2">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <f>VLOOKUP(B2,Sheet1!A:E,4, FALSE)</f>
+        <v>3.2514562800000001E-2</v>
+      </c>
+      <c r="H2" s="2">
+        <v>22300</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1000</v>
+      </c>
+      <c r="J2" s="2">
+        <f>(H2/I2)</f>
+        <v>22.3</v>
+      </c>
+      <c r="K2" s="2">
+        <f>J2*I2/60</f>
+        <v>371.66666666666669</v>
+      </c>
+      <c r="L2" s="2">
+        <v>300</v>
+      </c>
+      <c r="M2" s="2">
+        <v>248</v>
+      </c>
+      <c r="N2" s="2">
+        <f xml:space="preserve"> K2/D2</f>
+        <v>11430.775463684435</v>
+      </c>
+      <c r="O2" s="2">
+        <f>N2^(1/3)</f>
+        <v>22.526405518224941</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="2">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <f>VLOOKUP(B3,Sheet1!A:E,4, FALSE)</f>
+        <v>1.6007683688170321E-2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>9000</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="J3" s="2">
+        <f>(G3/I3)</f>
+        <v>9</v>
+      </c>
+      <c r="K3" s="2">
+        <f>J3*I3/60</f>
+        <v>150</v>
+      </c>
+      <c r="N3" s="2">
+        <f xml:space="preserve"> K3/D3</f>
+        <v>9370.5</v>
+      </c>
+      <c r="O3" s="2">
+        <f>N3^(1/3)</f>
+        <v>21.082442361941631</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="2">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <f>VLOOKUP(B4,Sheet1!A:E,4, FALSE)</f>
+        <v>1.6007683688170321E-2</v>
+      </c>
+      <c r="G4" s="2">
+        <v>12000</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1000</v>
+      </c>
+      <c r="J4" s="2">
+        <f>(G4/I4)</f>
+        <v>12</v>
+      </c>
+      <c r="K4" s="2">
+        <f>J4*I4/60</f>
+        <v>200</v>
+      </c>
+      <c r="N4" s="2">
+        <f xml:space="preserve"> K4/D4</f>
+        <v>12494</v>
+      </c>
+      <c r="O4" s="2">
+        <f>N4^(1/3)</f>
+        <v>23.204230302715143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="2">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <f>VLOOKUP(B5,Sheet1!A:E,4, FALSE)</f>
+        <v>3.4826709499999997E-2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>36000</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="J5" s="2">
+        <f>(H5/I5)</f>
+        <v>36</v>
+      </c>
+      <c r="K5" s="2">
+        <f>J5*I5/60</f>
+        <v>600</v>
+      </c>
+      <c r="N5" s="2">
+        <f xml:space="preserve"> K5/D5</f>
+        <v>17228.15645273637</v>
+      </c>
+      <c r="O5" s="2">
+        <f>N5^(1/3)</f>
+        <v>25.827335395101766</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="2">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <f>VLOOKUP(B6,Sheet1!A:E,4, FALSE)</f>
+        <v>1.6007683688170321E-2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>30000</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1000</v>
+      </c>
+      <c r="J6" s="2">
+        <f>(H6/I6)</f>
+        <v>30</v>
+      </c>
+      <c r="K6" s="2">
+        <f>J6*I6/60</f>
+        <v>500</v>
+      </c>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <f>VLOOKUP(B7,Sheet1!A:E,4, FALSE)</f>
+        <v>1.6007683688170321E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>5800</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1000</v>
+      </c>
+      <c r="J7" s="2">
+        <f>(G7/I7)</f>
+        <v>5.8</v>
+      </c>
+      <c r="K7" s="2">
+        <f>J7*I7/60</f>
+        <v>96.666666666666671</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <f>IF(ISTEXT(B8), VLOOKUP(B8,Sheet1!A:E,4, FALSE), "")</f>
+        <v>3.2514562800000001E-2</v>
+      </c>
+      <c r="G8" s="2">
+        <v>11000</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1000</v>
+      </c>
+      <c r="J8" s="2">
+        <f>(G8/I8)</f>
+        <v>11</v>
+      </c>
+      <c r="K8" s="2">
+        <f>J8*I8/60</f>
+        <v>183.33333333333334</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="D9" s="2" t="str">
+        <f>IF(ISTEXT(B9), VLOOKUP(B9,Sheet1!A:E,4, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="D10" s="2" t="str">
+        <f>IF(ISTEXT(B10), VLOOKUP(B10,Sheet1!A:E,4, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="D11" s="2" t="str">
+        <f>IF(ISTEXT(B11), VLOOKUP(B11,Sheet1!A:E,4, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="D12" s="2" t="str">
+        <f>IF(ISTEXT(B12), VLOOKUP(B12,Sheet1!A:E,4, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="D13" s="2" t="str">
+        <f>IF(ISTEXT(B13), VLOOKUP(B13,Sheet1!A:E,4, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="D14" s="2" t="str">
+        <f>IF(ISTEXT(B14), VLOOKUP(B14,Sheet1!A:E,4, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="D15" s="2" t="str">
+        <f>IF(ISTEXT(B15), VLOOKUP(B15,Sheet1!A:E,4, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="D16" s="2" t="str">
+        <f>IF(ISTEXT(B16), VLOOKUP(B16,Sheet1!A:E,4, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="4:15">
+      <c r="D17" s="2" t="str">
+        <f>IF(ISTEXT(B17), VLOOKUP(B17,Sheet1!A:E,4, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="4:15">
+      <c r="D18" s="2" t="str">
+        <f>IF(ISTEXT(B18), VLOOKUP(B18,Sheet1!A:E,4, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="4:15">
+      <c r="D19" s="2" t="str">
+        <f>IF(ISTEXT(B19), VLOOKUP(B19,Sheet1!A:E,4, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="4:15">
+      <c r="D20" s="2" t="str">
+        <f>IF(ISTEXT(B20), VLOOKUP(B20,Sheet1!A:E,4, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+    </row>
+    <row r="21" spans="4:15">
+      <c r="D21" s="2" t="str">
+        <f>IF(ISTEXT(B21), VLOOKUP(B21,Sheet1!A:E,4, FALSE), "")</f>
+        <v/>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+    </row>
+    <row r="22" spans="4:15">
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="4:15">
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+    </row>
+    <row r="24" spans="4:15">
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+    </row>
+    <row r="25" spans="4:15">
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+    </row>
+    <row r="26" spans="4:15">
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+    </row>
+    <row r="27" spans="4:15">
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="4:15">
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="4:15">
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+    </row>
+    <row r="30" spans="4:15">
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+    </row>
+    <row r="31" spans="4:15">
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+    </row>
+    <row r="32" spans="4:15">
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+    </row>
+    <row r="33" spans="14:15">
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+    </row>
+    <row r="34" spans="14:15">
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+    </row>
+    <row r="35" spans="14:15">
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+    </row>
+    <row r="36" spans="14:15">
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+    </row>
+    <row r="37" spans="14:15">
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14">
+        <v>12800</v>
+      </c>
+      <c r="E14">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15">
+        <v>14000</v>
+      </c>
+      <c r="D15">
+        <v>11000</v>
+      </c>
+      <c r="E15">
+        <v>9200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>